<commit_message>
fix type test dataset, make column name for nillable categorical mref shorter
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1665" windowWidth="25605" windowHeight="14625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
     <t>xcategoricalmref_value</t>
   </si>
   <si>
-    <t>xcategoricalmrefnillable_value</t>
+    <t>xcatmrefnillable_value</t>
   </si>
 </sst>
 </file>
@@ -887,40 +887,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="24" customWidth="1"/>
-    <col min="39" max="39" width="23.42578125" customWidth="1"/>
-    <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" customWidth="1"/>
+    <col min="39" max="39" width="23.5" customWidth="1"/>
+    <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5382,9 +5382,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5450,12 +5450,12 @@
       <selection activeCell="A5" sqref="A5:A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -5508,14 +5508,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>147</v>
       </c>
@@ -5568,23 +5568,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6268,7 +6268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>143</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" s="3" t="s">
         <v>149</v>
       </c>
@@ -6658,7 +6658,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" s="3" t="s">
         <v>150</v>
       </c>

</xml_diff>